<commit_message>
se agrega interfaz de app en flutter
</commit_message>
<xml_diff>
--- a/datos/agenda.xlsx
+++ b/datos/agenda.xlsx
@@ -93,7 +93,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,6 +104,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -137,29 +143,29 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -537,7 +543,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="31.5" customFormat="1" s="4">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="33" customFormat="1" s="4">
       <c r="A4" s="5" t="s">
         <v>16</v>
       </c>

</xml_diff>